<commit_message>
Practica 5_6 hecha jajajajaja
</commit_message>
<xml_diff>
--- a/Practica_5_6/Excel Cuentas.xlsx
+++ b/Practica_5_6/Excel Cuentas.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Master Informatica\PGPI\repositorio\PGPIproject\Practica_5_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\PGPIproject\Practica_5_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,14 +165,14 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -456,7 +456,7 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
@@ -698,11 +698,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -752,7 +752,7 @@
         <v>3.6</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D13" si="0">(B3*C3)</f>
+        <f t="shared" ref="D3:D11" si="0">(B3*C3)</f>
         <v>0.9</v>
       </c>
     </row>
@@ -761,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="7">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C4" s="5">
         <f>1.5*24/100</f>
@@ -769,7 +769,7 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>3.5999999999999997E-2</v>
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="9">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C5" s="5">
         <f>10*24/100</f>
@@ -785,7 +785,7 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>0.48</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C6" s="5">
         <f>1*24/100</f>
@@ -801,7 +801,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>1.2E-2</v>
+        <v>2.3999999999999998E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>0.25</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ref="C3:C13" si="1">20*24/100</f>
+        <f t="shared" ref="C7:C9" si="1">20*24/100</f>
         <v>4.8</v>
       </c>
       <c r="D7" s="1">
@@ -841,7 +841,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="9">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="9">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C11" s="5">
         <f>10*24/100</f>
@@ -881,18 +881,18 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10">
         <f>SUM(D2:D11)</f>
-        <v>10.067999999999998</v>
+        <v>8.1059999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,13 +908,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:H3"/>
+  <dimension ref="D3:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D3">
@@ -928,11 +928,21 @@
         <v>68451.599166666667</v>
       </c>
       <c r="G3">
-        <v>10.68</v>
+        <f>Hoja2!D12</f>
+        <v>8.1059999999999999</v>
       </c>
       <c r="H3">
         <f>F3*G3</f>
-        <v>731063.07909999997</v>
+        <v>554868.66284500004</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <f>F3*G4</f>
+        <v>616064.39249999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>